<commit_message>
union de columnas si validacion
</commit_message>
<xml_diff>
--- a/modulo/id_empresa.xlsx
+++ b/modulo/id_empresa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\Disagro\Proyecto_I_Analisis_y_Diseno\modulo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79950C5E-F4F0-4F68-BE21-F0B6B79D1D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514A73FD-5493-40C9-AA0E-81BF7B2B6C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12420" yWindow="684" windowWidth="10272" windowHeight="12396" xr2:uid="{8B1FD255-8D79-4733-9BAC-727D78C1A472}"/>
+    <workbookView xWindow="348" yWindow="0" windowWidth="10272" windowHeight="12396" xr2:uid="{8B1FD255-8D79-4733-9BAC-727D78C1A472}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="90">
   <si>
-    <t>company</t>
-  </si>
-  <si>
     <t>Yodel</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>id_empresa</t>
+  </si>
+  <si>
+    <t>name_company</t>
   </si>
 </sst>
 </file>
@@ -688,17 +688,17 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -706,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -722,7 +722,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -730,7 +730,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -738,7 +738,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -746,7 +746,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -754,7 +754,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -762,7 +762,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -770,7 +770,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -778,7 +778,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -786,7 +786,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -794,7 +794,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -802,7 +802,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -810,7 +810,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -818,7 +818,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -826,7 +826,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -834,7 +834,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -842,7 +842,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -850,7 +850,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -858,7 +858,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -866,7 +866,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -874,7 +874,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -882,7 +882,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -890,7 +890,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -898,7 +898,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -906,7 +906,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -914,7 +914,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -922,7 +922,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -930,7 +930,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -938,7 +938,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -946,7 +946,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -954,7 +954,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -962,7 +962,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -970,7 +970,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -978,7 +978,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -986,7 +986,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -994,7 +994,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1002,7 +1002,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1010,7 +1010,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1018,7 +1018,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1026,7 +1026,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1034,7 +1034,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -1042,7 +1042,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1050,7 +1050,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -1058,7 +1058,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1066,7 +1066,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1074,7 +1074,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1082,7 +1082,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1090,7 +1090,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1098,7 +1098,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1106,7 +1106,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1114,7 +1114,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1122,7 +1122,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1130,7 +1130,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1138,7 +1138,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1146,7 +1146,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -1154,7 +1154,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1162,7 +1162,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1170,7 +1170,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1178,7 +1178,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1186,7 +1186,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1194,7 +1194,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -1202,7 +1202,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1210,7 +1210,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -1218,7 +1218,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -1226,7 +1226,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -1234,7 +1234,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1242,7 +1242,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -1250,7 +1250,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -1258,7 +1258,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -1266,7 +1266,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -1274,7 +1274,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1282,7 +1282,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1290,7 +1290,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1298,7 +1298,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1306,7 +1306,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1314,7 +1314,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1322,7 +1322,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1330,7 +1330,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -1338,7 +1338,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1346,7 +1346,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1354,7 +1354,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -1362,7 +1362,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1370,7 +1370,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1378,7 +1378,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1386,7 +1386,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -1394,7 +1394,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -1402,7 +1402,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -1410,7 +1410,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -1418,7 +1418,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -1426,7 +1426,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -1434,7 +1434,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -1442,7 +1442,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -1450,7 +1450,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -1458,7 +1458,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -1466,7 +1466,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -1474,7 +1474,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -1482,7 +1482,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -1490,7 +1490,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -1498,7 +1498,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.4.0 actualizacion de endpoint de "descarga de archivo"
</commit_message>
<xml_diff>
--- a/modulo/id_empresa.xlsx
+++ b/modulo/id_empresa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\Disagro\Proyecto_I_Analisis_y_Diseno\modulo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79950C5E-F4F0-4F68-BE21-F0B6B79D1D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8785BDAD-C5D8-4813-9D16-4A1B094EF068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12420" yWindow="684" windowWidth="10272" windowHeight="12396" xr2:uid="{8B1FD255-8D79-4733-9BAC-727D78C1A472}"/>
+    <workbookView xWindow="348" yWindow="0" windowWidth="10272" windowHeight="12396" xr2:uid="{8B1FD255-8D79-4733-9BAC-727D78C1A472}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="90">
   <si>
-    <t>company</t>
-  </si>
-  <si>
     <t>Yodel</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>id_empresa</t>
+  </si>
+  <si>
+    <t>name_company</t>
   </si>
 </sst>
 </file>
@@ -688,17 +688,17 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -706,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -722,7 +722,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -730,7 +730,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -738,7 +738,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -746,7 +746,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -754,7 +754,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -762,7 +762,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -770,7 +770,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -778,7 +778,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -786,7 +786,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -794,7 +794,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -802,7 +802,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -810,7 +810,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -818,7 +818,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -826,7 +826,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -834,7 +834,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -842,7 +842,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -850,7 +850,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -858,7 +858,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -866,7 +866,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -874,7 +874,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -882,7 +882,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -890,7 +890,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -898,7 +898,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -906,7 +906,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -914,7 +914,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -922,7 +922,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -930,7 +930,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -938,7 +938,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -946,7 +946,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -954,7 +954,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -962,7 +962,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -970,7 +970,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -978,7 +978,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -986,7 +986,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -994,7 +994,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1002,7 +1002,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1010,7 +1010,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1018,7 +1018,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1026,7 +1026,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1034,7 +1034,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -1042,7 +1042,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1050,7 +1050,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -1058,7 +1058,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1066,7 +1066,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1074,7 +1074,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1082,7 +1082,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1090,7 +1090,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1098,7 +1098,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1106,7 +1106,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1114,7 +1114,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1122,7 +1122,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1130,7 +1130,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1138,7 +1138,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1146,7 +1146,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -1154,7 +1154,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1162,7 +1162,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1170,7 +1170,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1178,7 +1178,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1186,7 +1186,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1194,7 +1194,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -1202,7 +1202,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1210,7 +1210,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -1218,7 +1218,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -1226,7 +1226,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -1234,7 +1234,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1242,7 +1242,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -1250,7 +1250,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -1258,7 +1258,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -1266,7 +1266,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -1274,7 +1274,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1282,7 +1282,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1290,7 +1290,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1298,7 +1298,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1306,7 +1306,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1314,7 +1314,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1322,7 +1322,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1330,7 +1330,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -1338,7 +1338,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1346,7 +1346,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1354,7 +1354,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -1362,7 +1362,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1370,7 +1370,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1378,7 +1378,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1386,7 +1386,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -1394,7 +1394,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -1402,7 +1402,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -1410,7 +1410,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -1418,7 +1418,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -1426,7 +1426,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -1434,7 +1434,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -1442,7 +1442,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -1450,7 +1450,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -1458,7 +1458,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -1466,7 +1466,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -1474,7 +1474,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -1482,7 +1482,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -1490,7 +1490,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -1498,7 +1498,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>